<commit_message>
EPBDS-11139 Add more tests for SmartRules min/max columns with full qualified class name
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11139_fixTypeNotFoundError.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11139_fixTypeNotFoundError.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\.openl\user-workspace\DEFAULT\EPBDS-11139-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB5BA5D-6D2E-416F-B77C-1CD9F07355A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F12717-5A48-44C9-97D2-42CC56341969}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{820E0D86-4B3F-4221-8B93-E906AC9B6CFF}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="24165" windowHeight="12495" xr2:uid="{820E0D86-4B3F-4221-8B93-E906AC9B6CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$C$8:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="40">
   <si>
     <t>Rule</t>
   </si>
@@ -93,26 +93,72 @@
     <t>Result</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Solution 1 </t>
-  </si>
-  <si>
-    <t>3. Solution  3</t>
-  </si>
-  <si>
-    <t>2. Solution  2</t>
-  </si>
-  <si>
     <t>SmartRules String giveAssureur_solution3(String offerName, Integer  departmentNumber, java.time.LocalDate date)</t>
   </si>
   <si>
     <t>Test giveAssureur_solution3</t>
+  </si>
+  <si>
+    <t>SmartRules String giveAssureur_solution2(String offerName, Integer  departmentNumber, java.time.LocalTime time)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>SmartRules String giveAssureur_solution1(String offerName, Integer  departmentNumber, java.time.LocalDateTime datetime)</t>
+  </si>
+  <si>
+    <t>Test giveAssureur_solution2</t>
+  </si>
+  <si>
+    <t>Test giveAssureur_solution1</t>
+  </si>
+  <si>
+    <t>Test giveAssureur_solution4</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11:00 AM</t>
+  </si>
+  <si>
+    <t>20:00 PM</t>
+  </si>
+  <si>
+    <t>2019-01-10T10:15:00Z[UTC]</t>
+  </si>
+  <si>
+    <t>2019-12-10T10:15:00Z[UTC]</t>
+  </si>
+  <si>
+    <t>2020-01-10T10:15:00Z[UTC]</t>
+  </si>
+  <si>
+    <t>2021-10-10T10:15:00Z[UTC]</t>
+  </si>
+  <si>
+    <t>2020-05-10T10:15:00Z[UTC]</t>
+  </si>
+  <si>
+    <t>SmartRules String giveAssureur_solution4(String offerName, Integer  departmentNumber, java.time.ZonedDateTime datetime)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +173,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,12 +192,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,42 +258,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{51011668-790D-4A9D-B2D4-0F6906B79F94}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{15AE1CEB-1049-46FF-8D5D-D283A5CFCE9E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -261,9 +322,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -301,7 +362,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -407,7 +468,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -557,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB4ADD5-8D3C-4B3C-89D8-7EE7A0FB0F6D}">
-  <dimension ref="A2:G71"/>
+  <dimension ref="A3:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,189 +631,590 @@
     <col min="3" max="3" width="47.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="48" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>43831</v>
+      </c>
+      <c r="F5" s="14">
+        <v>44562</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>43831</v>
+      </c>
+      <c r="F6" s="14">
+        <v>44562</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>44562</v>
+      </c>
+      <c r="F7" s="14">
+        <v>46023</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="9">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14">
+        <v>43831</v>
+      </c>
+      <c r="F8" s="14">
+        <v>44561</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
+        <v>45214</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
+      <c r="F19" s="6"/>
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
+      <c r="E20" s="16">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="13">
+        <v>1</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E60" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="11"/>
-      <c r="G60" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
+      <c r="E32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C33" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D61" s="4">
-        <v>1</v>
-      </c>
-      <c r="E61" s="5">
-        <v>43831</v>
-      </c>
-      <c r="F61" s="5">
-        <v>44562</v>
-      </c>
-      <c r="G61" s="4" t="s">
+      <c r="D33" s="9">
+        <v>1</v>
+      </c>
+      <c r="E33" s="17">
+        <v>43892</v>
+      </c>
+      <c r="F33" s="17">
+        <v>44076</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="4">
+      <c r="C34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="9">
+        <v>1</v>
+      </c>
+      <c r="E34" s="17">
+        <v>44258</v>
+      </c>
+      <c r="F34" s="17">
+        <v>44442</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="13">
+        <v>1</v>
+      </c>
+      <c r="D41" s="17">
+        <v>44258.75</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E62" s="5">
-        <v>43831</v>
-      </c>
-      <c r="F62" s="5">
-        <v>44562</v>
-      </c>
-      <c r="G62" s="4" t="s">
+      <c r="C46" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="9">
+        <v>1</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="9">
+        <v>1</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="4" t="s">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="4">
-        <v>1</v>
-      </c>
-      <c r="E63" s="5">
-        <v>44562</v>
-      </c>
-      <c r="F63" s="5">
-        <v>46023</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64" s="4">
-        <v>4</v>
-      </c>
-      <c r="E64" s="5">
-        <v>43831</v>
-      </c>
-      <c r="F64" s="5">
-        <v>44561</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" s="6">
-        <v>1</v>
-      </c>
-      <c r="D71" s="7">
-        <v>45214</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C54" s="2">
+        <v>1</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0"/>
-  <autoFilter ref="C8:E12" xr:uid="{ACE073FA-A505-4EE5-A06E-CD760D30696D}"/>
-  <mergeCells count="3">
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="B68:E68"/>
+  <mergeCells count="12">
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>